<commit_message>
REPORTGEN-1086: fix part of issue
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/ISO-5055 Full Detailed Report - OMG Technical Debt Edition.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/ISO-5055 Full Detailed Report - OMG Technical Debt Edition.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Cast\ReportGenerator\1.22.0\Templates\Application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22D32B2-8EC2-4AE4-B725-04FB92D48C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0604D4C-E4C2-40EA-A381-B7B848ACC44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>Application characteristics</t>
   </si>
   <si>
-    <t>Findings summary for CAST under OMG-ASCQM Standards</t>
-  </si>
-  <si>
     <t>Technology</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>RepGen:TABLE;TECHNICAL_SIZING;HEADER=NO</t>
   </si>
   <si>
-    <t>Quality Standard</t>
-  </si>
-  <si>
     <t>Rules</t>
   </si>
   <si>
@@ -137,27 +131,12 @@
     <t>ISO-5055 Compliance details</t>
   </si>
   <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=ISO-5055-Security,COUNT=-1,HEADER=NO</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=ISO-5055-Reliability,COUNT=-1,HEADER=NO</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=ISO-5055-Maintainability,COUNT=-1,HEADER=NO</t>
-  </si>
-  <si>
-    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=ISO-5055-Performance-Efficiency,COUNT=-1,HEADER=NO</t>
-  </si>
-  <si>
     <t>ISO Technical Debt:</t>
   </si>
   <si>
     <t>RepGen:TEXT;OMG_TECHNICAL_DEBT</t>
   </si>
   <si>
-    <t>RepGen:TABLE;OMG_TECHNICAL_DEBT_EVOLUTION;ID=ISO-5055-Index,HEADER=NO</t>
-  </si>
-  <si>
     <t>Technical Debt (Days)</t>
   </si>
   <si>
@@ -177,6 +156,27 @@
   </si>
   <si>
     <t>RepGen:TABLE;OMG_TECHNICAL_DEBT_RULES_EVOLUTION;ID=ISO-5055-Security,DESC=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>Findings summary for CAST under ISO-5055 Standards</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;OMG_TECHNICAL_DEBT_EVOLUTION;ID=ISO-5055-Index,MORE=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>ISO-5055</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=ISO-5055-Security,COUNT=-1,HEADER=NO,OMG=true</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=ISO-5055-Reliability,COUNT=-1,HEADER=NO,OMG=true</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=ISO-5055-Performance-Efficiency,COUNT=-1,HEADER=NO,OMG=true</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=ISO-5055-Maintainability,COUNT=-1,HEADER=NO,OMG=true</t>
   </si>
 </sst>
 </file>
@@ -837,7 +837,7 @@
   <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +868,7 @@
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="2"/>
@@ -902,10 +902,10 @@
       <c r="D4" s="4"/>
       <c r="E4" s="13"/>
       <c r="F4" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -916,29 +916,29 @@
         <v>8</v>
       </c>
       <c r="C6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>10</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="23"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>13</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="23"/>
       <c r="N9" s="17"/>
@@ -946,26 +946,26 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="19" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -1002,30 +1002,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1045,7 +1045,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,33 +1062,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1118,30 +1118,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1178,33 +1178,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1234,30 +1234,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1277,7 +1277,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,33 +1294,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1350,30 +1350,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1393,7 +1393,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,33 +1410,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>